<commit_message>
sua doi ke hoach
</commit_message>
<xml_diff>
--- a/kehoach.xlsx
+++ b/kehoach.xlsx
@@ -55,9 +55,6 @@
     <t>Thiết kế Class Bảng Băm</t>
   </si>
   <si>
-    <t>Thực hiện phần đọc file input.txt</t>
-  </si>
-  <si>
     <t>Thiết kế Form MainScreen</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Thực hiện chức năng tra từ liên kết với bảng băm</t>
+  </si>
+  <si>
+    <t>Thực hiện phần đọc dữ liệu từ trong SQL</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,13 +599,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F5" s="5">
         <v>43110</v>
@@ -622,7 +622,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5">
         <v>43141</v>
@@ -638,10 +638,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="5">
@@ -662,7 +662,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="5">
         <v>43141</v>
@@ -678,10 +678,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="5">
@@ -698,17 +698,17 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="5">
         <v>43383</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -718,17 +718,17 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="5">
         <v>43383</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -738,17 +738,17 @@
         <v>8</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="5">
         <v>43383</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -758,17 +758,17 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="5">
         <v>43383</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -778,17 +778,17 @@
         <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="5">
         <v>43383</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -798,17 +798,17 @@
         <v>11</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="5">
         <v>43383</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -818,19 +818,19 @@
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="5">
         <v>43383</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -840,19 +840,19 @@
         <v>13</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="5">
         <v>43383</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -862,10 +862,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="5">
@@ -882,19 +882,19 @@
         <v>15</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="5">
         <v>43384</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -904,19 +904,19 @@
         <v>16</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>

</xml_diff>

<commit_message>
cap nhat thoi gian lam viec - kehoach.xlsx
</commit_message>
<xml_diff>
--- a/kehoach.xlsx
+++ b/kehoach.xlsx
@@ -198,9 +198,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -211,9 +216,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -523,7 +525,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,64 +540,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -619,7 +621,7 @@
       <c r="G5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="9">
         <v>43110</v>
       </c>
     </row>
@@ -627,7 +629,7 @@
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3"/>
@@ -640,10 +642,10 @@
       <c r="F6" s="5">
         <v>43353</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="9">
         <v>43291</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="9">
         <v>43291</v>
       </c>
     </row>
@@ -651,7 +653,7 @@
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -664,14 +666,18 @@
       <c r="F7" s="5">
         <v>43353</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="9">
+        <v>43200</v>
+      </c>
+      <c r="H7" s="9">
+        <v>43322</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3"/>
@@ -684,16 +690,16 @@
       <c r="F8" s="5">
         <v>43353</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="9">
         <v>43291</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -706,14 +712,18 @@
       <c r="F9" s="5">
         <v>43353</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="9">
+        <v>43322</v>
+      </c>
+      <c r="H9" s="9">
+        <v>43322</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3"/>
@@ -726,14 +736,14 @@
       <c r="F10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="3"/>
@@ -746,14 +756,14 @@
       <c r="F11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="3"/>
@@ -766,14 +776,14 @@
       <c r="F12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3"/>
@@ -786,14 +796,14 @@
       <c r="F13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="3"/>
@@ -806,14 +816,14 @@
       <c r="F14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -826,14 +836,14 @@
       <c r="F15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -848,14 +858,14 @@
       <c r="F16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>13</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -870,14 +880,14 @@
       <c r="F17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -890,14 +900,14 @@
       <c r="F18" s="5">
         <v>43354</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>15</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -912,14 +922,14 @@
       <c r="F19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>16</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -934,18 +944,18 @@
       <c r="F20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Them form tra tu, ham tra tu, cap nhat ke hoach ngay 19/10/2018
</commit_message>
<xml_diff>
--- a/kehoach.xlsx
+++ b/kehoach.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>KẾ HOẠCH ĐỒ ÁN ỨNG DỤNG BẢNG BĂM LÀM TỪ ĐIỂN</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>28/09/2018</t>
+  </si>
+  <si>
+    <t>19/10/2018</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,9 +864,7 @@
       <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="5">
         <v>43383</v>
       </c>
@@ -880,9 +881,7 @@
       <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>22</v>
       </c>
@@ -892,8 +891,12 @@
       <c r="F17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="G17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">

</xml_diff>

<commit_message>
update ke hoach, ham Search, ham Delete
</commit_message>
<xml_diff>
--- a/kehoach.xlsx
+++ b/kehoach.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>KẾ HOẠCH ĐỒ ÁN ỨNG DỤNG BẢNG BĂM LÀM TỪ ĐIỂN</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Thiết kế Form Add, Delete, Edit, Option</t>
   </si>
   <si>
-    <t>Thiết kế Form History và Form Information</t>
-  </si>
-  <si>
     <t>Thiết kế phần nghe từ</t>
   </si>
   <si>
@@ -116,6 +113,12 @@
   </si>
   <si>
     <t>19/10/2018</t>
+  </si>
+  <si>
+    <t>Thiết kế Form Information</t>
+  </si>
+  <si>
+    <t>20/10/2018</t>
   </si>
 </sst>
 </file>
@@ -610,19 +613,19 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="F5" s="5">
         <v>43110</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="9">
         <v>43110</v>
@@ -637,7 +640,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5">
         <v>43141</v>
@@ -657,10 +660,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="5">
@@ -685,7 +688,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="5">
         <v>43141</v>
@@ -705,10 +708,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="5">
@@ -733,18 +736,20 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="5">
         <v>43383</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="9">
         <v>43444</v>
       </c>
-      <c r="H10" s="8"/>
+      <c r="H10" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -755,18 +760,20 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="5">
         <v>43383</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="9">
         <v>43444</v>
       </c>
-      <c r="H11" s="8"/>
+      <c r="H11" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -777,79 +784,85 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="5">
         <v>43383</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="9">
         <v>43444</v>
       </c>
-      <c r="H12" s="8"/>
+      <c r="H12" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="5">
         <v>43383</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="9">
         <v>43444</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="5">
         <v>43383</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="9">
         <v>43444</v>
       </c>
-      <c r="H14" s="8"/>
+      <c r="H14" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>11</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="5">
         <v>43383</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -859,17 +872,17 @@
         <v>12</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="5">
         <v>43383</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -879,23 +892,23 @@
         <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" s="5">
         <v>43383</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -903,10 +916,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="5">
@@ -923,19 +936,19 @@
         <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="5">
         <v>43384</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -945,19 +958,19 @@
         <v>16</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>

</xml_diff>

<commit_message>
chinh sua ham edit, ham add, ham search, ham delete
</commit_message>
<xml_diff>
--- a/kehoach.xlsx
+++ b/kehoach.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>KẾ HOẠCH ĐỒ ÁN ỨNG DỤNG BẢNG BĂM LÀM TỪ ĐIỂN</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>20/10/2018</t>
+  </si>
+  <si>
+    <t>15/10/2018</t>
+  </si>
+  <si>
+    <t>30/10/2018</t>
   </si>
 </sst>
 </file>
@@ -531,7 +537,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,8 +890,12 @@
       <c r="F16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="G16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">

</xml_diff>

<commit_message>
cap nhat tinh hinh ke hoach
</commit_message>
<xml_diff>
--- a/kehoach.xlsx
+++ b/kehoach.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>KẾ HOẠCH ĐỒ ÁN ỨNG DỤNG BẢNG BĂM LÀM TỪ ĐIỂN</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>30/10/2018</t>
+  </si>
+  <si>
+    <t>25/10/2018</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,8 +873,12 @@
       <c r="F15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="G15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">

</xml_diff>

<commit_message>
sua loi khong cap nhat comboboxedit sau khi xoa tu
</commit_message>
<xml_diff>
--- a/kehoach.xlsx
+++ b/kehoach.xlsx
@@ -540,7 +540,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,8 +945,12 @@
       <c r="F18" s="5">
         <v>43354</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="9">
+        <v>43111</v>
+      </c>
+      <c r="H18" s="9">
+        <v>43415</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">

</xml_diff>

<commit_message>
cap nhat ke hoach
</commit_message>
<xml_diff>
--- a/kehoach.xlsx
+++ b/kehoach.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t>KẾ HOẠCH ĐỒ ÁN ỨNG DỤNG BẢNG BĂM LÀM TỪ ĐIỂN</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>25/10/2018</t>
+  </si>
+  <si>
+    <t>Lịch sử tra từ</t>
+  </si>
+  <si>
+    <t>14/11/2018</t>
   </si>
 </sst>
 </file>
@@ -198,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -219,6 +225,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -537,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,64 +564,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -953,33 +962,35 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="10">
         <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="5">
-        <v>43384</v>
+      <c r="E19" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+        <v>39</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>16</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>21</v>
@@ -987,24 +998,46 @@
       <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>25</v>
+      <c r="E20" s="5">
+        <v>43384</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>